<commit_message>
Before the rework of ripping out mysql
</commit_message>
<xml_diff>
--- a/analysis/cmg_predictions_2018-02-10.xlsx
+++ b/analysis/cmg_predictions_2018-02-10.xlsx
@@ -684,7 +684,7 @@
         <v>43144</v>
       </c>
       <c r="C35">
-        <v>315.0986911040941</v>
+        <v>310.0673573678168</v>
       </c>
       <c r="D35">
         <v>12619931607415.22</v>
@@ -695,7 +695,7 @@
         <v>43145</v>
       </c>
       <c r="C36">
-        <v>283.578184842342</v>
+        <v>278.3624022107832</v>
       </c>
       <c r="D36">
         <v>12619931607383.78</v>
@@ -706,7 +706,7 @@
         <v>43146</v>
       </c>
       <c r="C37">
-        <v>284.4437142794281</v>
+        <v>276.3235210340654</v>
       </c>
       <c r="D37">
         <v>39309016569680.94</v>

</xml_diff>